<commit_message>
Update ReadMe and added files in Load folder
</commit_message>
<xml_diff>
--- a/Transform/data_notes.xlsx
+++ b/Transform/data_notes.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jabuk\Documents\USC_DataScience\ETL Project\COVID19_Repo\COVID19-ETL-Project\Transform\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32231A3D-AEA3-48F9-B77F-9CE7BAAC64BF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5E69A8C-0355-4DB2-87D1-54A3AD11D10B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="525" windowWidth="22695" windowHeight="14565" xr2:uid="{6F4DDC7F-A36F-47DA-86C6-EF9544E6DAE2}"/>
+    <workbookView xWindow="1905" yWindow="165" windowWidth="22785" windowHeight="14565" xr2:uid="{6F4DDC7F-A36F-47DA-86C6-EF9544E6DAE2}"/>
   </bookViews>
   <sheets>
     <sheet name="KM-notes" sheetId="1" r:id="rId1"/>
-    <sheet name="county_ids" sheetId="2" r:id="rId2"/>
+    <sheet name="unique_county" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="219">
   <si>
     <t>county</t>
   </si>
@@ -689,6 +689,9 @@
   </si>
   <si>
     <t>make the primary key because it has the most records of counties</t>
+  </si>
+  <si>
+    <t>counties</t>
   </si>
 </sst>
 </file>
@@ -750,7 +753,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -798,11 +801,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -831,6 +843,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1145,10 +1158,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21C918CC-0137-4B5D-A821-79E0900D7702}">
-  <dimension ref="A1:L75"/>
+  <dimension ref="A1:M75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" topLeftCell="C58" workbookViewId="0">
+      <selection activeCell="O50" sqref="O50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1537,8 +1550,11 @@
       <c r="B32" t="s">
         <v>7</v>
       </c>
+      <c r="C32" t="s">
+        <v>55</v>
+      </c>
       <c r="H32" s="16" t="s">
-        <v>24</v>
+        <v>218</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -1562,6 +1578,9 @@
       <c r="B34" t="s">
         <v>7</v>
       </c>
+      <c r="C34" t="s">
+        <v>55</v>
+      </c>
       <c r="F34" s="2" t="s">
         <v>22</v>
       </c>
@@ -1590,6 +1609,9 @@
       <c r="B36" t="s">
         <v>7</v>
       </c>
+      <c r="C36" t="s">
+        <v>55</v>
+      </c>
       <c r="F36" s="2" t="s">
         <v>25</v>
       </c>
@@ -1602,7 +1624,7 @@
         <v>7</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H37" s="16" t="s">
         <v>25</v>
@@ -1615,8 +1637,11 @@
       <c r="B38" t="s">
         <v>7</v>
       </c>
+      <c r="C38" t="s">
+        <v>55</v>
+      </c>
       <c r="F38" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="H38" s="17" t="s">
         <v>0</v>
@@ -1630,7 +1655,7 @@
         <v>7</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="H39" s="17" t="s">
         <v>5</v>
@@ -1643,8 +1668,11 @@
       <c r="B40" t="s">
         <v>7</v>
       </c>
+      <c r="C40" t="s">
+        <v>55</v>
+      </c>
       <c r="F40" s="2" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H40" s="17" t="s">
         <v>25</v>
@@ -1658,10 +1686,10 @@
         <v>7</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="H41" s="17" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -1671,11 +1699,11 @@
       <c r="B42" t="s">
         <v>7</v>
       </c>
+      <c r="C42" t="s">
+        <v>55</v>
+      </c>
       <c r="F42" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H42" s="17" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -1685,126 +1713,79 @@
       <c r="B43" t="s">
         <v>7</v>
       </c>
-      <c r="F43" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="H43" s="17" t="s">
-        <v>34</v>
-      </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>38</v>
       </c>
-      <c r="F44" s="2" t="s">
-        <v>33</v>
+      <c r="C44" t="s">
+        <v>55</v>
+      </c>
+      <c r="H44" s="16" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F45" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H45" s="16" t="s">
+      <c r="H45" s="17" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H46" s="17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H47" s="17" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F46" s="2" t="s">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H48" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="H46" s="17" t="s">
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H52" s="16" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H53" s="17" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F47" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="H47" s="17" t="s">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H54" s="17" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F48" s="2" t="s">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H55" s="17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H56" s="17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H57" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="H48" s="17" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F49" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="H49" s="17" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H50" s="17" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H51" s="17" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H53" s="16" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H54" s="17" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H55" s="17" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H56" s="17" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H57" s="17" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H58" s="17" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H59" s="17" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H60" s="17" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H61" s="17" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F62" s="4"/>
-      <c r="G62" s="5"/>
-      <c r="H62" s="18"/>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M61" s="5"/>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G62" s="20"/>
       <c r="I62" s="5"/>
       <c r="J62" s="5"/>
       <c r="K62" s="5"/>
       <c r="L62" s="5"/>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>58</v>
       </c>
@@ -1814,16 +1795,16 @@
       <c r="C63" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F63" s="6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>68</v>
       </c>
       <c r="C64" t="s">
         <v>55</v>
+      </c>
+      <c r="F64" s="6" t="s">
+        <v>58</v>
       </c>
       <c r="H64" s="16" t="s">
         <v>215</v>
@@ -1836,9 +1817,6 @@
       <c r="C65" t="s">
         <v>55</v>
       </c>
-      <c r="F65" s="2" t="s">
-        <v>59</v>
-      </c>
       <c r="H65" s="17" t="s">
         <v>0</v>
       </c>
@@ -1851,7 +1829,7 @@
         <v>4</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>5</v>
+        <v>59</v>
       </c>
       <c r="H66" s="19" t="s">
         <v>5</v>
@@ -1865,7 +1843,7 @@
         <v>5</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>62</v>
+        <v>5</v>
       </c>
       <c r="H67" s="17" t="s">
         <v>64</v>
@@ -1879,7 +1857,7 @@
         <v>55</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H68" s="17" t="s">
         <v>65</v>
@@ -1893,7 +1871,7 @@
         <v>55</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H69" s="17" t="s">
         <v>66</v>
@@ -1904,7 +1882,7 @@
         <v>62</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H70" s="17" t="s">
         <v>67</v>
@@ -1918,7 +1896,7 @@
         <v>69</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
@@ -1927,6 +1905,9 @@
       </c>
       <c r="B72" t="s">
         <v>7</v>
+      </c>
+      <c r="F72" s="2" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update readme, revise vaccine data & data_notes
</commit_message>
<xml_diff>
--- a/Transform/data_notes.xlsx
+++ b/Transform/data_notes.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jabuk\Documents\USC_DataScience\ETL Project\COVID19_Repo\COVID19-ETL-Project\Transform\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5E69A8C-0355-4DB2-87D1-54A3AD11D10B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0893DC09-AB91-43D4-881E-604CBB93F914}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1905" yWindow="165" windowWidth="22785" windowHeight="14565" xr2:uid="{6F4DDC7F-A36F-47DA-86C6-EF9544E6DAE2}"/>
+    <workbookView xWindow="5070" yWindow="15" windowWidth="22485" windowHeight="14565" firstSheet="1" activeTab="1" xr2:uid="{6F4DDC7F-A36F-47DA-86C6-EF9544E6DAE2}"/>
   </bookViews>
   <sheets>
     <sheet name="KM-notes" sheetId="1" r:id="rId1"/>
-    <sheet name="unique_county" sheetId="2" r:id="rId2"/>
+    <sheet name="unique_counties" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="242">
   <si>
     <t>county</t>
   </si>
@@ -685,13 +685,82 @@
     <t>employment/unemployment data</t>
   </si>
   <si>
-    <t>Counties with population from this data file</t>
-  </si>
-  <si>
     <t>make the primary key because it has the most records of counties</t>
   </si>
   <si>
     <t>counties</t>
+  </si>
+  <si>
+    <t>Primary Key Basis</t>
+  </si>
+  <si>
+    <t>Outside CA</t>
+  </si>
+  <si>
+    <t>only 1 record in 3/12/2021</t>
+  </si>
+  <si>
+    <t>only 1 record in 3/10/2021</t>
+  </si>
+  <si>
+    <t>2 records in 3/9/2021 &amp; 3/3/2021</t>
+  </si>
+  <si>
+    <t>2 records in 3/9/2021 &amp; 2/9/2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Morgan </t>
+  </si>
+  <si>
+    <t>only 1 record in 3/5/2021</t>
+  </si>
+  <si>
+    <t>2 records in 3/4/2021 &amp; 2/4/2021</t>
+  </si>
+  <si>
+    <t>2 records in 3/4/2021 &amp; 2/11/2021</t>
+  </si>
+  <si>
+    <t>only 1 record in 3/4/2021</t>
+  </si>
+  <si>
+    <t>2 records in 3/3/2021 &amp; 2/10/2021</t>
+  </si>
+  <si>
+    <t>only 1 record in 3/3/2021</t>
+  </si>
+  <si>
+    <t>only 1 record in 3/2/2021</t>
+  </si>
+  <si>
+    <t>2 records in 3/1/2021 &amp; 1/31/2021</t>
+  </si>
+  <si>
+    <t>only 1 record in 2/25/2021</t>
+  </si>
+  <si>
+    <t>only 1 record in 2/19/2021</t>
+  </si>
+  <si>
+    <t>only 1 record in 2/18/2021</t>
+  </si>
+  <si>
+    <t>3 records in 2/17, 1/26 &amp; 1/6/2021</t>
+  </si>
+  <si>
+    <t>2 records in 2/17 &amp; 2/11/2021</t>
+  </si>
+  <si>
+    <t>2 records in 1/19 &amp; 12/29/2020</t>
+  </si>
+  <si>
+    <t>58 Counties in CA</t>
+  </si>
+  <si>
+    <t>Resources: Wikipedia</t>
+  </si>
+  <si>
+    <t>Counties&lt;&gt;Vaccine data</t>
   </si>
 </sst>
 </file>
@@ -814,7 +883,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -844,6 +913,13 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1160,7 +1236,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21C918CC-0137-4B5D-A821-79E0900D7702}">
   <dimension ref="A1:M75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C58" workbookViewId="0">
+    <sheetView topLeftCell="C58" workbookViewId="0">
       <selection activeCell="O50" sqref="O50"/>
     </sheetView>
   </sheetViews>
@@ -1219,7 +1295,7 @@
         <v>0</v>
       </c>
       <c r="I5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -1554,7 +1630,7 @@
         <v>55</v>
       </c>
       <c r="H32" s="16" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -1942,985 +2018,1317 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2234D7C-1EDF-4D18-9F2A-FAD1111A2737}">
-  <dimension ref="A1:G85"/>
+  <dimension ref="A1:H86"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="C89" sqref="C89"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.5703125" customWidth="1"/>
-    <col min="7" max="7" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" customWidth="1"/>
+    <col min="2" max="2" width="25" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="23.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="F1" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="22" t="s">
+        <v>153</v>
+      </c>
+      <c r="B2" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C2" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="12" t="s">
-        <v>153</v>
-      </c>
-      <c r="G1" s="14" t="s">
+      <c r="D2" s="25" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="9"/>
-      <c r="C2" s="7"/>
-      <c r="E2" s="12"/>
-      <c r="G2" s="14"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="F2" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="12"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="14"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="B4" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="C4" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="G3" s="15" t="s">
+      <c r="D4" s="15" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="F4" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="G4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="B5" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="D5" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="F5" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="G4" s="15" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+      <c r="G5" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="B6" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="D6" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="F6" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="G5" s="15" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+      <c r="G6" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="B7" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C7" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="D7" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="F7" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="G6" s="15" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+      <c r="G7" t="s">
+        <v>116</v>
+      </c>
+      <c r="H7" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="B8" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C8" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="D8" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="F8" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="G7" s="15" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+      <c r="G8" t="s">
+        <v>134</v>
+      </c>
+      <c r="H8" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="B9" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C9" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="E8" s="13" t="s">
-        <v>154</v>
-      </c>
-      <c r="G8" s="15" t="s">
+      <c r="D9" s="15" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
+      <c r="F9" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="G9" t="s">
+        <v>81</v>
+      </c>
+      <c r="H9" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="B10" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C10" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="D10" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="G10" t="s">
+        <v>140</v>
+      </c>
+      <c r="H10" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="G11" t="s">
+        <v>148</v>
+      </c>
+      <c r="H11" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="G12" t="s">
+        <v>77</v>
+      </c>
+      <c r="H12" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="B13" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="G9" s="15" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="C10" s="8" t="s">
+      <c r="C13" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>166</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="G13" t="s">
+        <v>135</v>
+      </c>
+      <c r="H13" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="G14" t="s">
+        <v>224</v>
+      </c>
+      <c r="H14" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="G15" t="s">
+        <v>86</v>
+      </c>
+      <c r="H15" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="G16" t="s">
+        <v>96</v>
+      </c>
+      <c r="H16" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="B17" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="E10" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="G10" s="15" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
+      <c r="C17" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="G17" t="s">
+        <v>147</v>
+      </c>
+      <c r="H17" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="G18" t="s">
+        <v>73</v>
+      </c>
+      <c r="H18" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="G19" t="s">
+        <v>91</v>
+      </c>
+      <c r="H19" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="G20" t="s">
+        <v>76</v>
+      </c>
+      <c r="H20" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>174</v>
+      </c>
+      <c r="F21" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="G21" t="s">
+        <v>87</v>
+      </c>
+      <c r="H21" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="F22" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="G22" t="s">
+        <v>100</v>
+      </c>
+      <c r="H22" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>176</v>
+      </c>
+      <c r="F23" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="G23" t="s">
+        <v>99</v>
+      </c>
+      <c r="H23" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="F24" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="G24" t="s">
+        <v>105</v>
+      </c>
+      <c r="H24" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>178</v>
+      </c>
+      <c r="F25" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="G25" t="s">
+        <v>92</v>
+      </c>
+      <c r="H25" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="D26" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="F26" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="G26" t="s">
+        <v>95</v>
+      </c>
+      <c r="H26" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="D27" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="G27" t="s">
+        <v>103</v>
+      </c>
+      <c r="H27" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D28" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="F28" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="G28" t="s">
+        <v>149</v>
+      </c>
+      <c r="H28" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="D29" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="F29" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="G29" t="s">
         <v>78</v>
       </c>
-      <c r="C11" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="E11" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="G11" s="15" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="E12" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="G12" s="15" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="E13" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="G13" s="15" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="E14" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="G14" s="15" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="E15" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="G15" s="15" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="E16" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="G16" s="15" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="E17" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="G17" s="15" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="C18" s="8" t="s">
+      <c r="H29" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="D30" s="15" t="s">
+        <v>183</v>
+      </c>
+      <c r="F30" s="12" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="B31" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="E18" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="G18" s="15" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="C19" s="8" t="s">
+      <c r="C31" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="D31" s="15" t="s">
+        <v>184</v>
+      </c>
+      <c r="F31" s="12" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="B32" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="E19" s="13" t="s">
-        <v>94</v>
-      </c>
-      <c r="G19" s="15" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="C20" s="8" t="s">
+      <c r="C32" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="D32" s="15" t="s">
+        <v>185</v>
+      </c>
+      <c r="F32" s="12" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="D33" s="15" t="s">
+        <v>186</v>
+      </c>
+      <c r="F33" s="12" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="D34" s="15" t="s">
+        <v>187</v>
+      </c>
+      <c r="F34" s="12" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="B35" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="E20" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="G20" s="15" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="C21" s="8" t="s">
+      <c r="C35" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="D35" s="15" t="s">
+        <v>188</v>
+      </c>
+      <c r="F35" s="12" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="B36" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="E21" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="G21" s="15" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="C22" s="8" t="s">
+      <c r="C36" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="D36" s="15" t="s">
+        <v>189</v>
+      </c>
+      <c r="F36" s="12" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="B37" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="D37" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="F37" s="12" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="B38" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="E22" s="13" t="s">
-        <v>101</v>
-      </c>
-      <c r="G22" s="15" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="C23" s="8" t="s">
+      <c r="C38" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="D38" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="F38" s="12" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="B39" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="E23" s="13" t="s">
-        <v>102</v>
-      </c>
-      <c r="G23" s="15" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="C24" s="8" t="s">
+      <c r="C39" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="D39" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="F39" s="12" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="B40" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="D40" s="15" t="s">
+        <v>193</v>
+      </c>
+      <c r="F40" s="12" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="B41" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="E24" s="13" t="s">
-        <v>104</v>
-      </c>
-      <c r="G24" s="15" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="C25" s="8" t="s">
+      <c r="C41" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="D41" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="F41" s="12" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B42" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="E25" s="13" t="s">
-        <v>152</v>
-      </c>
-      <c r="G25" s="15" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="C26" s="8" t="s">
+      <c r="C42" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="D42" s="15" t="s">
+        <v>195</v>
+      </c>
+      <c r="F42" s="12" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="B43" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="E26" s="13" t="s">
-        <v>106</v>
-      </c>
-      <c r="G26" s="15" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="C27" s="8" t="s">
+      <c r="C43" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="D43" s="15" t="s">
+        <v>196</v>
+      </c>
+      <c r="F43" s="12" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="B44" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="E27" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="G27" s="15" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="C28" s="8" t="s">
+      <c r="C44" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="D44" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="F44" s="12" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="B45" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="E28" s="13" t="s">
-        <v>108</v>
-      </c>
-      <c r="G28" s="15" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="C29" s="8" t="s">
+      <c r="C45" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="D45" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="F45" s="12" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="B46" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="C46" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="D46" s="15" t="s">
+        <v>199</v>
+      </c>
+      <c r="F46" s="12" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="B47" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="E29" s="13" t="s">
-        <v>109</v>
-      </c>
-      <c r="G29" s="15" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="C30" s="8" t="s">
+      <c r="C47" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="D47" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="F47" s="12" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="B48" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="E30" s="13" t="s">
-        <v>110</v>
-      </c>
-      <c r="G30" s="15" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="C31" s="8" t="s">
+      <c r="C48" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="D48" s="15" t="s">
+        <v>201</v>
+      </c>
+      <c r="F48" s="12" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="B49" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="E31" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="G31" s="15" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="C32" s="8" t="s">
+      <c r="C49" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="D49" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="F49" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="B50" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="C50" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="D50" s="15" t="s">
+        <v>203</v>
+      </c>
+      <c r="F50" s="12" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="B51" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="C51" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="D51" s="15" t="s">
+        <v>204</v>
+      </c>
+      <c r="F51" s="12" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="B52" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="E32" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="G32" s="15" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="C33" s="8" t="s">
+      <c r="C52" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="D52" s="15" t="s">
+        <v>205</v>
+      </c>
+      <c r="F52" s="12" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="B53" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="E33" s="13" t="s">
-        <v>114</v>
-      </c>
-      <c r="G33" s="15" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="C34" s="8" t="s">
+      <c r="C53" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="D53" s="15" t="s">
+        <v>206</v>
+      </c>
+      <c r="F53" s="12" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="B54" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="E34" s="13" t="s">
-        <v>155</v>
-      </c>
-      <c r="G34" s="15" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="C35" s="8" t="s">
+      <c r="C54" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D54" s="15" t="s">
+        <v>207</v>
+      </c>
+      <c r="F54" s="12" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="B55" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="E35" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="G35" s="15" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="C36" s="8" t="s">
+      <c r="C55" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="D55" s="15" t="s">
+        <v>208</v>
+      </c>
+      <c r="F55" s="12" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="B56" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="E36" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="G36" s="15" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="C37" s="8" t="s">
+      <c r="C56" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="D56" s="15" t="s">
+        <v>209</v>
+      </c>
+      <c r="F56" s="12" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="B57" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="E37" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="G37" s="15" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="10" t="s">
-        <v>152</v>
-      </c>
-      <c r="C38" s="8" t="s">
+      <c r="C57" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="D57" s="15" t="s">
+        <v>210</v>
+      </c>
+      <c r="F57" s="12" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="B58" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="E38" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="G38" s="15" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="C39" s="8" t="s">
+      <c r="C58" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="D58" s="15" t="s">
+        <v>211</v>
+      </c>
+      <c r="F58" s="12" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="B59" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="E39" s="13" t="s">
-        <v>121</v>
-      </c>
-      <c r="G39" s="15" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="C40" s="8" t="s">
+      <c r="C59" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="D59" s="15" t="s">
+        <v>212</v>
+      </c>
+      <c r="F59" s="12" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="B60" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="E40" s="13" t="s">
-        <v>122</v>
-      </c>
-      <c r="G40" s="15" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="C41" s="8" t="s">
+      <c r="D60" s="15" t="s">
+        <v>213</v>
+      </c>
+      <c r="F60" s="12" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="B61" s="10" t="s">
         <v>126</v>
       </c>
-      <c r="E41" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="G41" s="15" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="C42" s="8" t="s">
+      <c r="D61" s="15" t="s">
+        <v>214</v>
+      </c>
+      <c r="F61" s="12" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="B62" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="E42" s="13" t="s">
-        <v>124</v>
-      </c>
-      <c r="G42" s="15" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="C43" s="8" t="s">
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="B63" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="E43" s="13" t="s">
-        <v>125</v>
-      </c>
-      <c r="G43" s="15" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="C44" s="8" t="s">
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="11"/>
+      <c r="B64" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="E44" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="G44" s="15" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="C45" s="8" t="s">
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="21"/>
+      <c r="B65" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="E45" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="G45" s="15" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="C46" s="8" t="s">
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B66" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="E46" s="13" t="s">
-        <v>128</v>
-      </c>
-      <c r="G46" s="15" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="C47" s="8" t="s">
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B67" s="10" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B68" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="E47" s="13" t="s">
-        <v>129</v>
-      </c>
-      <c r="G47" s="15" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="C48" s="8" t="s">
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B69" s="10" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B70" s="10" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B71" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="E48" s="13" t="s">
-        <v>130</v>
-      </c>
-      <c r="G48" s="15" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="C49" s="8" t="s">
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B72" s="10" t="s">
         <v>137</v>
       </c>
-      <c r="E49" s="13" t="s">
-        <v>131</v>
-      </c>
-      <c r="G49" s="15" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="C50" s="8" t="s">
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B73" s="10" t="s">
         <v>138</v>
       </c>
-      <c r="E50" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="G50" s="15" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="C51" s="8" t="s">
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B74" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="E51" s="13" t="s">
-        <v>133</v>
-      </c>
-      <c r="G51" s="15" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="C52" s="8" t="s">
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B75" s="10" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B76" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="E52" s="13" t="s">
-        <v>136</v>
-      </c>
-      <c r="G52" s="15" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="C53" s="8" t="s">
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B77" s="10" t="s">
         <v>142</v>
       </c>
-      <c r="E53" s="13" t="s">
-        <v>137</v>
-      </c>
-      <c r="G53" s="15" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="C54" s="8" t="s">
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B78" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="E54" s="13" t="s">
-        <v>138</v>
-      </c>
-      <c r="G54" s="15" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="C55" s="8" t="s">
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B79" s="10" t="s">
         <v>144</v>
       </c>
-      <c r="E55" s="13" t="s">
-        <v>139</v>
-      </c>
-      <c r="G55" s="15" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="C56" s="8" t="s">
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B80" s="10" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B81" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="E56" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="G56" s="15" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="C57" s="8" t="s">
+    </row>
+    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B82" s="10" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B83" s="10" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B84" s="10" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B85" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="E57" s="13" t="s">
-        <v>142</v>
-      </c>
-      <c r="G57" s="15" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="10" t="s">
-        <v>124</v>
-      </c>
-      <c r="C58" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="E58" s="13" t="s">
-        <v>143</v>
-      </c>
-      <c r="G58" s="15" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="10" t="s">
-        <v>125</v>
-      </c>
-      <c r="E59" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="G59" s="15" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" s="10" t="s">
-        <v>126</v>
-      </c>
-      <c r="E60" s="13" t="s">
-        <v>145</v>
-      </c>
-      <c r="G60" s="15" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="E61" s="13" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="E62" s="13" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="E63" s="13" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="E64" s="11"/>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="E65" s="13" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="10" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="10" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="10" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="10" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="10" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="10" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="10" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="10" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" s="10" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" s="10" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="10" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" s="10" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78" s="10" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A79" s="10" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A80" s="10" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A81" s="10" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A82" s="10" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A83" s="10" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A84" s="10" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A85" s="10" t="s">
+    </row>
+    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B86" s="10" t="s">
         <v>151</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>